<commit_message>
Update consensus results comparison
</commit_message>
<xml_diff>
--- a/results_lgbm/compare_with_ibes/#compare_all.xlsx
+++ b/results_lgbm/compare_with_ibes/#compare_all.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ibes_ex_fwd</t>
   </si>
@@ -431,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -665,20 +665,6 @@
         <v>0.007461367279642713</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13">
-        <v>0.008869719261200689</v>
-      </c>
-      <c r="F13">
-        <v>9000</v>
-      </c>
-      <c r="I13">
-        <v>0.009339954370972705</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update consensus / dense
</commit_message>
<xml_diff>
--- a/results_lgbm/compare_with_ibes/#compare_all.xlsx
+++ b/results_lgbm/compare_with_ibes/#compare_all.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Clair/PycharmProjects/ai_value/results_lgbm/compare_with_ibes/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8464F251-A363-FA4C-85AA-EF5D7049F62B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="average" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">average!$A$1:$D$19</definedName>
+  </definedNames>
+  <calcPr calcId="191029" iterateDelta="9.9999999999994451E-4"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>consensus</t>
   </si>
@@ -28,6 +47,9 @@
     <t>index</t>
   </si>
   <si>
+    <t>ibes_6_ni</t>
+  </si>
+  <si>
     <t>ibes_2_ni</t>
   </si>
   <si>
@@ -43,12 +65,24 @@
     <t>ibes_6_niqcut</t>
   </si>
   <si>
+    <t>ibes_1_fwdepsqcut_dense</t>
+  </si>
+  <si>
+    <t>ni_2_niqcut</t>
+  </si>
+  <si>
+    <t>ni_6_fwdeps</t>
+  </si>
+  <si>
     <t>ni_1_epsqcut</t>
   </si>
   <si>
     <t>ni_2_epsqcut</t>
   </si>
   <si>
+    <t>ni_2_fwdeps</t>
+  </si>
+  <si>
     <t>ni_1_fwdepsqcut</t>
   </si>
   <si>
@@ -59,13 +93,19 @@
   </si>
   <si>
     <t>ni_6_fwdepsqcut</t>
+  </si>
+  <si>
+    <t>ni_6_niqcut</t>
+  </si>
+  <si>
+    <t>ibes_2_niqcut</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +117,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,17 +172,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -174,7 +241,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -206,9 +273,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,6 +325,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -415,14 +518,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="249" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -436,161 +545,272 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.008604109548964898</v>
+        <v>7.4774416114006493E-3</v>
       </c>
       <c r="C2">
-        <v>14467</v>
+        <v>568</v>
       </c>
       <c r="D2">
-        <v>0.007461390831007631</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>6.9521974415974377E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.008604109548964898</v>
+        <v>8.6041095489648983E-3</v>
       </c>
       <c r="C3">
         <v>14467</v>
       </c>
       <c r="D3">
-        <v>0.007470316543135013</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>7.4613908310076308E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.008604109548964898</v>
+        <v>8.6041095489648983E-3</v>
       </c>
       <c r="C4">
         <v>14467</v>
       </c>
       <c r="D4">
-        <v>0.008215291392886251</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>7.4703165431350129E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.008610171467262949</v>
+        <v>8.6041095489648983E-3</v>
       </c>
       <c r="C5">
+        <v>14467</v>
+      </c>
+      <c r="D5">
+        <v>8.2152913928862509E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3">
+        <v>8.6101714672629486E-3</v>
+      </c>
+      <c r="C6" s="3">
         <v>13776</v>
       </c>
-      <c r="D5">
-        <v>0.008239669139180731</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>0.008673141980908865</v>
-      </c>
-      <c r="C6">
-        <v>13402</v>
-      </c>
-      <c r="D6">
-        <v>0.008290320575140078</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6" s="3">
+        <v>8.239669139180731E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7">
-        <v>0.00930690016118596</v>
+        <v>8.6731419809088651E-3</v>
       </c>
       <c r="C7">
-        <v>14467</v>
+        <v>13402</v>
       </c>
       <c r="D7">
-        <v>0.01322805762894923</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
+        <v>8.2903205751400783E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
-        <v>0.009384087290453671</v>
-      </c>
-      <c r="C8">
-        <v>14289</v>
-      </c>
-      <c r="D8">
-        <v>0.01340126360609522</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="B8" s="3">
+        <v>8.6589441840465731E-3</v>
+      </c>
+      <c r="C8" s="3">
+        <v>11650</v>
+      </c>
+      <c r="D8" s="3">
+        <v>9.0657110962312683E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9">
-        <v>0.00930690016118596</v>
+        <v>8.5283509711310858E-3</v>
       </c>
       <c r="C9">
-        <v>14467</v>
+        <v>2695</v>
       </c>
       <c r="D9">
-        <v>0.01367246194968542</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>1.262906986070185E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10">
-        <v>0.009384087290453671</v>
+        <v>9.038742197873241E-3</v>
       </c>
       <c r="C10">
-        <v>14289</v>
+        <v>4248</v>
       </c>
       <c r="D10">
-        <v>0.01373872658434699</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>1.26430822285556E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11">
-        <v>0.009486213628492479</v>
+        <v>9.3069001611859603E-3</v>
       </c>
       <c r="C11">
-        <v>14246</v>
+        <v>14467</v>
       </c>
       <c r="D11">
-        <v>0.01400753774994666</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>1.3228057628949229E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B12">
-        <v>0.009492788784155153</v>
+        <v>9.3840872904536708E-3</v>
       </c>
       <c r="C12">
+        <v>14289</v>
+      </c>
+      <c r="D12">
+        <v>1.3401263606095219E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>8.6448079918162533E-3</v>
+      </c>
+      <c r="C13">
+        <v>8817</v>
+      </c>
+      <c r="D13">
+        <v>1.3415102948218131E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>9.3069001611859603E-3</v>
+      </c>
+      <c r="C14">
+        <v>14467</v>
+      </c>
+      <c r="D14">
+        <v>1.3672461949685419E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>9.3840872904536708E-3</v>
+      </c>
+      <c r="C15">
+        <v>14289</v>
+      </c>
+      <c r="D15">
+        <v>1.3738726584346991E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>9.4862136284924788E-3</v>
+      </c>
+      <c r="C16">
+        <v>14246</v>
+      </c>
+      <c r="D16">
+        <v>1.4007537749946661E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>9.4927887841551525E-3</v>
+      </c>
+      <c r="C17">
         <v>14279</v>
       </c>
-      <c r="D12">
-        <v>0.01403873064787338</v>
+      <c r="D17">
+        <v>1.4038730647873379E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>1.2284657043992781E-2</v>
+      </c>
+      <c r="C18">
+        <v>172</v>
+      </c>
+      <c r="D18">
+        <v>1.536086770476644E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>8.0573748375082702E-3</v>
+      </c>
+      <c r="C19">
+        <v>9416</v>
+      </c>
+      <c r="D19">
+        <v>0.1837138298836869</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D19" xr:uid="{6095B2EB-9B77-2946-AF56-03942DB49ED8}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="11650"/>
+        <filter val="13402"/>
+        <filter val="13776"/>
+        <filter val="14246"/>
+        <filter val="14279"/>
+        <filter val="14289"/>
+        <filter val="14467"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update preprocess / LightGBM.py
</commit_message>
<xml_diff>
--- a/results_lgbm/compare_with_ibes/#compare_all.xlsx
+++ b/results_lgbm/compare_with_ibes/#compare_all.xlsx
@@ -1,39 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Clair/PycharmProjects/ai_value/results_lgbm/compare_with_ibes/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8464F251-A363-FA4C-85AA-EF5D7049F62B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="average" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">average!$A$1:$D$19</definedName>
-  </definedNames>
-  <calcPr calcId="191029" iterateDelta="9.9999999999994451E-4"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>consensus</t>
   </si>
@@ -56,6 +37,9 @@
     <t>ibes_2_fwdeps</t>
   </si>
   <si>
+    <t>ibes_2_fwdepsqcut_ibes_new industry_monthly</t>
+  </si>
+  <si>
     <t>ibes_2_fwdepsqcut</t>
   </si>
   <si>
@@ -63,6 +47,9 @@
   </si>
   <si>
     <t>ibes_6_niqcut</t>
+  </si>
+  <si>
+    <t>ibes_1_fwdepsqcut_dense_small</t>
   </si>
   <si>
     <t>ibes_1_fwdepsqcut_dense</t>
@@ -104,8 +91,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,21 +104,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,29 +144,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -241,7 +201,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -273,27 +233,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -325,24 +267,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -518,20 +442,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="249" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -545,272 +463,301 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>7.4774416114006493E-3</v>
+        <v>0.007477441611400649</v>
       </c>
       <c r="C2">
         <v>568</v>
       </c>
       <c r="D2">
-        <v>6.9521974415974377E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.006952197441597438</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>8.6041095489648983E-3</v>
+        <v>0.008604109548964898</v>
       </c>
       <c r="C3">
         <v>14467</v>
       </c>
       <c r="D3">
-        <v>7.4613908310076308E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.007461390831007631</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8.6041095489648983E-3</v>
+        <v>0.008604109548964898</v>
       </c>
       <c r="C4">
         <v>14467</v>
       </c>
       <c r="D4">
-        <v>7.4703165431350129E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.007470316543135013</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>8.6041095489648983E-3</v>
+        <v>0.008085902054067038</v>
       </c>
       <c r="C5">
+        <v>8620</v>
+      </c>
+      <c r="D5">
+        <v>0.007745530837691133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.008604109548964898</v>
+      </c>
+      <c r="C6">
         <v>14467</v>
       </c>
-      <c r="D5">
-        <v>8.2152913928862509E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="3">
-        <v>8.6101714672629486E-3</v>
-      </c>
-      <c r="C6" s="3">
-        <v>13776</v>
-      </c>
-      <c r="D6" s="3">
-        <v>8.239669139180731E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>0.008215291392886251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7">
-        <v>8.6731419809088651E-3</v>
+        <v>0.008610171467262949</v>
       </c>
       <c r="C7">
+        <v>13776</v>
+      </c>
+      <c r="D7">
+        <v>0.008239669139180731</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0.008673141980908865</v>
+      </c>
+      <c r="C8">
         <v>13402</v>
       </c>
-      <c r="D7">
-        <v>8.2903205751400783E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="3">
-        <v>8.6589441840465731E-3</v>
-      </c>
-      <c r="C8" s="3">
-        <v>11650</v>
-      </c>
-      <c r="D8" s="3">
-        <v>9.0657110962312683E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>0.008290320575140078</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9">
-        <v>8.5283509711310858E-3</v>
+        <v>0.008579285668533483</v>
       </c>
       <c r="C9">
-        <v>2695</v>
+        <v>6736</v>
       </c>
       <c r="D9">
-        <v>1.262906986070185E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>0.009053436204286813</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10">
-        <v>9.038742197873241E-3</v>
+        <v>0.008658944184046573</v>
       </c>
       <c r="C10">
+        <v>11650</v>
+      </c>
+      <c r="D10">
+        <v>0.009065711096231268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>0.008658944184046573</v>
+      </c>
+      <c r="C11">
+        <v>11650</v>
+      </c>
+      <c r="D11">
+        <v>0.009065711096231268</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>0.008528350971131086</v>
+      </c>
+      <c r="C12">
+        <v>2695</v>
+      </c>
+      <c r="D12">
+        <v>0.01262906986070185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>0.009038742197873241</v>
+      </c>
+      <c r="C13">
         <v>4248</v>
       </c>
-      <c r="D10">
-        <v>1.26430822285556E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>9.3069001611859603E-3</v>
-      </c>
-      <c r="C11">
-        <v>14467</v>
-      </c>
-      <c r="D11">
-        <v>1.3228057628949229E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>9.3840872904536708E-3</v>
-      </c>
-      <c r="C12">
-        <v>14289</v>
-      </c>
-      <c r="D12">
-        <v>1.3401263606095219E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="D13">
+        <v>0.0126430822285556</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13">
-        <v>8.6448079918162533E-3</v>
-      </c>
-      <c r="C13">
-        <v>8817</v>
-      </c>
-      <c r="D13">
-        <v>1.3415102948218131E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="B14">
-        <v>9.3069001611859603E-3</v>
+        <v>0.00930690016118596</v>
       </c>
       <c r="C14">
         <v>14467</v>
       </c>
       <c r="D14">
-        <v>1.3672461949685419E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.01322805762894923</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>9.3840872904536708E-3</v>
+        <v>0.009384087290453671</v>
       </c>
       <c r="C15">
         <v>14289</v>
       </c>
       <c r="D15">
-        <v>1.3738726584346991E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.01340126360609522</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>0.008644807991816253</v>
+      </c>
+      <c r="C16">
+        <v>8817</v>
+      </c>
+      <c r="D16">
+        <v>0.01341510294821813</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16">
-        <v>9.4862136284924788E-3</v>
-      </c>
-      <c r="C16">
+      <c r="B17">
+        <v>0.00930690016118596</v>
+      </c>
+      <c r="C17">
+        <v>14467</v>
+      </c>
+      <c r="D17">
+        <v>0.01367246194968542</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>0.009384087290453671</v>
+      </c>
+      <c r="C18">
+        <v>14289</v>
+      </c>
+      <c r="D18">
+        <v>0.01373872658434699</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>0.009486213628492479</v>
+      </c>
+      <c r="C19">
         <v>14246</v>
       </c>
-      <c r="D16">
-        <v>1.4007537749946661E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17">
-        <v>9.4927887841551525E-3</v>
-      </c>
-      <c r="C17">
+      <c r="D19">
+        <v>0.01400753774994666</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>0.009492788784155153</v>
+      </c>
+      <c r="C20">
         <v>14279</v>
       </c>
-      <c r="D17">
-        <v>1.4038730647873379E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18">
-        <v>1.2284657043992781E-2</v>
-      </c>
-      <c r="C18">
+      <c r="D20">
+        <v>0.01403873064787338</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>0.01228465704399278</v>
+      </c>
+      <c r="C21">
         <v>172</v>
       </c>
-      <c r="D18">
-        <v>1.536086770476644E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19">
-        <v>8.0573748375082702E-3</v>
-      </c>
-      <c r="C19">
+      <c r="D21">
+        <v>0.01536086770476644</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>0.00805737483750827</v>
+      </c>
+      <c r="C22">
         <v>9416</v>
       </c>
-      <c r="D19">
+      <c r="D22">
         <v>0.1837138298836869</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D19" xr:uid="{6095B2EB-9B77-2946-AF56-03942DB49ED8}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="11650"/>
-        <filter val="13402"/>
-        <filter val="13776"/>
-        <filter val="14246"/>
-        <filter val="14279"/>
-        <filter val="14289"/>
-        <filter val="14467"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>